<commit_message>
Fix Exception when end of sheet not detected
</commit_message>
<xml_diff>
--- a/testfiles/entrada/new/ModeloGerado.xlsx
+++ b/testfiles/entrada/new/ModeloGerado.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="59">
   <si>
     <t>Título:</t>
   </si>
@@ -79,6 +79,9 @@
   </si>
   <si>
     <t/>
+  </si>
+  <si>
+    <t>0</t>
   </si>
   <si>
     <t>0386841901</t>
@@ -477,47 +480,47 @@
         <v>21</v>
       </c>
       <c r="J7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" t="s">
+        <v>21</v>
+      </c>
+      <c r="I8" t="s">
+        <v>21</v>
+      </c>
+      <c r="J8" t="s">
         <v>22</v>
-      </c>
-      <c r="B8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F8" t="s">
-        <v>21</v>
-      </c>
-      <c r="G8" t="s">
-        <v>21</v>
-      </c>
-      <c r="H8" t="s">
-        <v>21</v>
-      </c>
-      <c r="I8" t="s">
-        <v>21</v>
-      </c>
-      <c r="J8" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C9" t="s">
         <v>19</v>
@@ -541,15 +544,15 @@
         <v>21</v>
       </c>
       <c r="J9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C10" t="s">
         <v>19</v>
@@ -573,15 +576,15 @@
         <v>21</v>
       </c>
       <c r="J10" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C11" t="s">
         <v>19</v>
@@ -605,15 +608,15 @@
         <v>21</v>
       </c>
       <c r="J11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C12" t="s">
         <v>19</v>
@@ -637,15 +640,15 @@
         <v>21</v>
       </c>
       <c r="J12" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B13" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C13" t="s">
         <v>19</v>
@@ -669,15 +672,15 @@
         <v>21</v>
       </c>
       <c r="J13" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C14" t="s">
         <v>19</v>
@@ -701,7 +704,7 @@
         <v>21</v>
       </c>
       <c r="J14" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -774,10 +777,10 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C7" t="s">
         <v>19</v>
@@ -788,10 +791,10 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C8" t="s">
         <v>20</v>
@@ -802,10 +805,10 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B9" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C9" t="s">
         <v>19</v>
@@ -816,10 +819,10 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B10" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C10" t="s">
         <v>19</v>
@@ -830,10 +833,10 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B11" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C11" t="s">
         <v>19</v>
@@ -844,10 +847,10 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B12" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C12" t="s">
         <v>19</v>
@@ -858,10 +861,10 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B13" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C13" t="s">
         <v>19</v>
@@ -872,10 +875,10 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C14" t="s">
         <v>19</v>
@@ -886,10 +889,10 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C15" t="s">
         <v>19</v>
@@ -900,10 +903,10 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B16" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C16" t="s">
         <v>19</v>
@@ -914,10 +917,10 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B17" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C17" t="s">
         <v>19</v>

</xml_diff>